<commit_message>
Nice 2 have update
</commit_message>
<xml_diff>
--- a/seating_arrangement.xlsx
+++ b/seating_arrangement.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Nathalie</t>
+          <t xml:space="preserve">Ivan </t>
         </is>
       </c>
     </row>
@@ -468,7 +468,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Jens</t>
+          <t>Caroline</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Daryoush</t>
+          <t>Nasrin</t>
         </is>
       </c>
     </row>
@@ -502,7 +502,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Em</t>
+          <t>Gerrit</t>
         </is>
       </c>
     </row>
@@ -519,7 +519,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Mahsa</t>
+          <t>Jens</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Gerrit</t>
+          <t>Viktor</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Yanina</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Andrea</t>
+          <t>Dario</t>
         </is>
       </c>
     </row>
@@ -604,7 +604,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ivan </t>
+          <t>Niels</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Caroline</t>
+          <t>Mahsa</t>
         </is>
       </c>
     </row>
@@ -638,7 +638,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Danil</t>
+          <t>Ariana</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Sweta</t>
+          <t>Nathalie</t>
         </is>
       </c>
     </row>
@@ -672,7 +672,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Karel</t>
+          <t>Andrea</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Fabienne</t>
+          <t>Em</t>
         </is>
       </c>
     </row>
@@ -706,7 +706,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Yanina</t>
+          <t>Alexander</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Nasrin</t>
+          <t>Danil</t>
         </is>
       </c>
     </row>
@@ -757,177 +757,42 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Ariana</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Table 5</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Seat 1</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Viktor</t>
+          <t>Miguel</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Table 5</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Seat 2</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Niels</t>
+          <t>Remaining Colleagues:</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Table 5</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Seat 3</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Geraldine</t>
+          <t>Sweta</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Table 5</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Seat 4</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Miguel</t>
+          <t>Karel</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Table 5</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Seat 5</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Empty</t>
+          <t>Fabienne</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Table 6</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Seat 1</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Empty</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Table 6</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Seat 2</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Empty</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Table 6</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Seat 3</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Empty</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Table 6</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Seat 4</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Empty</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Table 6</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Seat 5</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Empty</t>
+          <t>Geraldine</t>
         </is>
       </c>
     </row>

</xml_diff>